<commit_message>
KIBON-917: Lastenausgleich Excel Export: Erste Version noch ohne Totals
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
@@ -8,22 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\P$\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E20D3FD-D095-47DB-A47D-3075018A388C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B3AB88-CDDE-4021-BFCB-5331D143A7B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17835" xr2:uid="{6D37441E-09CE-4F94-BF5A-8FAE3F6E6CF7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{1AEF1F9C-938D-450B-BF9F-74AAB8E05F65}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="anteil">Data!#REF!</definedName>
-    <definedName name="eingabeLastenausgleich">Data!$H$9</definedName>
-    <definedName name="gutschein">Data!#REF!</definedName>
-    <definedName name="kostenPro100ProzentPlatz">Data!$F$9</definedName>
-    <definedName name="selbstbehaltGemeinde">Data!$G$9</definedName>
-    <definedName name="totalBelegung">Data!$D$9</definedName>
-    <definedName name="totalGutscheine">Data!$E$9</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +31,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+  <si>
+    <t>Lastenausgleich</t>
+  </si>
   <si>
     <t>Parameter</t>
   </si>
@@ -48,40 +42,49 @@
     <t>Jahr</t>
   </si>
   <si>
+    <t>{berechnungsjahr}</t>
+  </si>
+  <si>
+    <t>Kantonal durchschnittlicher Selbstbehalt pro 100% Platz im Vorjahr</t>
+  </si>
+  <si>
+    <t>Gemeinde</t>
+  </si>
+  <si>
+    <t>BFS-Nummer</t>
+  </si>
+  <si>
+    <t>Total Belegung</t>
+  </si>
+  <si>
+    <t>Total Gutscheine</t>
+  </si>
+  <si>
+    <t>Kosten pro 100% Platz</t>
+  </si>
+  <si>
+    <t>Selbstbehalt Gemeinde</t>
+  </si>
+  <si>
+    <t>Eingabe Lastenausgleich</t>
+  </si>
+  <si>
+    <t>Korrektur</t>
+  </si>
+  <si>
     <t>{repeatRow}</t>
   </si>
   <si>
-    <t>Kosten pro 100% Platz</t>
-  </si>
-  <si>
-    <t>Lastenausgleich</t>
-  </si>
-  <si>
-    <t>Kantonal durchschnittliche Kosten pro 100% Platz im Vorjahr</t>
-  </si>
-  <si>
-    <t>{berechnungsjahr}</t>
-  </si>
-  <si>
-    <t>{kostenPro100ProzentPlatz}</t>
-  </si>
-  <si>
-    <t>Gemeinde</t>
-  </si>
-  <si>
-    <t>BFS-Nummer</t>
-  </si>
-  <si>
-    <t>Total Belegung</t>
-  </si>
-  <si>
-    <t>Total Gutscheine</t>
-  </si>
-  <si>
-    <t>Selbstbehalt Gemeinde</t>
-  </si>
-  <si>
-    <t>Eingabe Lastenausgleich</t>
+    <t>{gemeinde}</t>
+  </si>
+  <si>
+    <t>{bfsNummer}</t>
+  </si>
+  <si>
+    <t>{verrechnungsjahr}</t>
+  </si>
+  <si>
+    <t>{korrektur}</t>
   </si>
   <si>
     <t>{totalBelegung}</t>
@@ -96,28 +99,36 @@
     <t>{eingabeLastenausgleich}</t>
   </si>
   <si>
-    <t>{verrechnungsjahr}</t>
-  </si>
-  <si>
-    <t>{durchschnittlicheKostenPro100ProzentPlatz}</t>
-  </si>
-  <si>
-    <t>{gemeinde}</t>
-  </si>
-  <si>
-    <t>{bfsNummer}</t>
+    <t>{selbstbehaltProHundertProzentPlatz}</t>
+  </si>
+  <si>
+    <t>{kostenProHundertProzentPlatz}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$CHF-807]\ #,##0.00"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$CHF-807]\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -132,8 +143,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -149,18 +159,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -183,73 +193,36 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -561,155 +534,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFD2C01-3190-4613-9E97-C1D328FAAE82}">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0BAB2BE-640F-45EA-ADC8-77B8E625E64E}">
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="56" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="F8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="10">
-        <f>SUM(totalBelegung)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="11">
-        <f>SUM(totalGutscheine)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="11">
-        <f>SUM(kostenPro100ProzentPlatz)</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="11">
-        <f>SUM(selbstbehaltGemeinde)</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="11">
-        <f>SUM(eingabeLastenausgleich)</f>
-        <v>0</v>
-      </c>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="B7:B8"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
KIBON-917: Lastenausgleich Excel Export: Mit Totals
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
@@ -8,13 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\P$\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B3AB88-CDDE-4021-BFCB-5331D143A7B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FC28DF-8B8D-457B-9403-3F8D859E96F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{1AEF1F9C-938D-450B-BF9F-74AAB8E05F65}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="eingabeLastenausgleich">Data!$H$8</definedName>
+    <definedName name="kostenProHundertProzentPlatz">Data!$F$8</definedName>
+    <definedName name="selbstbehaltGemeinde">Data!$G$8</definedName>
+    <definedName name="totalBelegung">Data!$D$8</definedName>
+    <definedName name="totalGutscheine">Data!$E$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -537,9 +544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0BAB2BE-640F-45EA-ADC8-77B8E625E64E}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -639,11 +644,26 @@
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="D9" s="9">
+        <f>SUM(totalBelegung)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="10">
+        <f>SUM(totalGutscheine)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <f>SUM(kostenProHundertProzentPlatz)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <f>SUM(selbstbehaltGemeinde)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
+        <f>SUM(eingabeLastenausgleich)</f>
+        <v>0</v>
+      </c>
       <c r="I9" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KIBON-917: Lastenausgleich Excel Export: Korrekturen aus Vorjahren berechnen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\P$\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FC28DF-8B8D-457B-9403-3F8D859E96F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2643421E-486D-4E82-824B-6AA27D980A29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{1AEF1F9C-938D-450B-BF9F-74AAB8E05F65}"/>
   </bookViews>
@@ -17,6 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="eingabeLastenausgleich">Data!$H$8</definedName>
+    <definedName name="korrektur">Data!$I$8</definedName>
     <definedName name="kostenProHundertProzentPlatz">Data!$F$8</definedName>
     <definedName name="selbstbehaltGemeinde">Data!$G$8</definedName>
     <definedName name="totalBelegung">Data!$D$8</definedName>
@@ -120,13 +121,7 @@
     <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$CHF-807]\ #,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,38 +196,180 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -549,7 +686,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="11" style="3"/>
+    <col min="2" max="2" width="15.75" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11" style="3"/>
+    <col min="4" max="4" width="15.25" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
@@ -618,19 +762,19 @@
       <c r="C8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="8" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="8" t="s">
@@ -652,10 +796,7 @@
         <f>SUM(totalGutscheine)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="10">
-        <f>SUM(kostenProHundertProzentPlatz)</f>
-        <v>0</v>
-      </c>
+      <c r="F9" s="10"/>
       <c r="G9" s="10">
         <f>SUM(selbstbehaltGemeinde)</f>
         <v>0</v>

</xml_diff>

<commit_message>
KIBON-917: Lastenausgleich Excel Export: Formatierung der Felder in Excel
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\P$\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2643421E-486D-4E82-824B-6AA27D980A29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FC7590-BF76-483D-8545-198410490ECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{1AEF1F9C-938D-450B-BF9F-74AAB8E05F65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17835" xr2:uid="{1AEF1F9C-938D-450B-BF9F-74AAB8E05F65}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -199,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -219,157 +219,13 @@
     <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -762,19 +618,19 @@
       <c r="C8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="12" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="8" t="s">

</xml_diff>

<commit_message>
KIBON-1664: Excel erweitert + 2 Sprachig
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\P$\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FC7590-BF76-483D-8545-198410490ECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B12A345-E979-4D49-B7CA-3FBA3F1F6FA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17835" xr2:uid="{1AEF1F9C-938D-450B-BF9F-74AAB8E05F65}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1AEF1F9C-938D-450B-BF9F-74AAB8E05F65}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,13 @@
   <definedNames>
     <definedName name="eingabeLastenausgleich">Data!$H$8</definedName>
     <definedName name="korrektur">Data!$I$8</definedName>
+    <definedName name="kostenFuerSelbstbehalt">Data!$L$8</definedName>
     <definedName name="kostenProHundertProzentPlatz">Data!$F$8</definedName>
     <definedName name="selbstbehaltGemeinde">Data!$G$8</definedName>
     <definedName name="totalBelegung">Data!$D$8</definedName>
+    <definedName name="totalBelegungOhneSelbstbehalt">Data!$J$8</definedName>
     <definedName name="totalGutscheine">Data!$E$8</definedName>
+    <definedName name="totalGutscheineOhneSelbstbehalt">Data!$K$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +34,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,47 +45,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
-  <si>
-    <t>Lastenausgleich</t>
-  </si>
-  <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>Jahr</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>{berechnungsjahr}</t>
   </si>
   <si>
-    <t>Kantonal durchschnittlicher Selbstbehalt pro 100% Platz im Vorjahr</t>
-  </si>
-  <si>
-    <t>Gemeinde</t>
-  </si>
-  <si>
-    <t>BFS-Nummer</t>
-  </si>
-  <si>
-    <t>Total Belegung</t>
-  </si>
-  <si>
-    <t>Total Gutscheine</t>
-  </si>
-  <si>
-    <t>Kosten pro 100% Platz</t>
-  </si>
-  <si>
-    <t>Selbstbehalt Gemeinde</t>
-  </si>
-  <si>
-    <t>Eingabe Lastenausgleich</t>
-  </si>
-  <si>
-    <t>Korrektur</t>
-  </si>
-  <si>
     <t>{repeatRow}</t>
   </si>
   <si>
@@ -111,6 +81,63 @@
   </si>
   <si>
     <t>{kostenProHundertProzentPlatz}</t>
+  </si>
+  <si>
+    <t>{totalBelegungOhneSelbstbehalt}</t>
+  </si>
+  <si>
+    <t>{totalGutscheineOhneSelbstbehalt}</t>
+  </si>
+  <si>
+    <t>{kostenFuerSelbstbehalt}</t>
+  </si>
+  <si>
+    <t>{lastenausgleichTitel}</t>
+  </si>
+  <si>
+    <t>{parameterTitle}</t>
+  </si>
+  <si>
+    <t>{jahrTitel}</t>
+  </si>
+  <si>
+    <t>{selbstbehaltProHundertProzentPlatzTitel}</t>
+  </si>
+  <si>
+    <t>{gemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{bfsNummerTitel}</t>
+  </si>
+  <si>
+    <t>{totalBelegungTitel}</t>
+  </si>
+  <si>
+    <t>{totalGutscheineTitel}</t>
+  </si>
+  <si>
+    <t>{belegungenMitSelbstbehaltTitel}</t>
+  </si>
+  <si>
+    <t>{kostenProPlatzTitel}</t>
+  </si>
+  <si>
+    <t>{selbstbehaltGemeindeTitel}</t>
+  </si>
+  <si>
+    <t>{eingabeLastenausgleichTitel}</t>
+  </si>
+  <si>
+    <t>{korrekturTitle}</t>
+  </si>
+  <si>
+    <t>{belegungenOhneSelbstbehaltTitel}</t>
+  </si>
+  <si>
+    <t>{totalGutscheineEingabeLastTitel}</t>
+  </si>
+  <si>
+    <t>{kostenFuerSelbstbehaltTitel}</t>
   </si>
 </sst>
 </file>
@@ -121,12 +148,19 @@
     <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$CHF-807]\ #,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -172,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -195,32 +229,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -535,135 +628,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0BAB2BE-640F-45EA-ADC8-77B8E625E64E}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="56" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.75" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.59765625" style="3" customWidth="1"/>
     <col min="3" max="3" width="11" style="3"/>
-    <col min="4" max="4" width="15.25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.59765625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.09765625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="20.09765625" style="3" customWidth="1"/>
     <col min="8" max="8" width="17.5" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="11" style="3"/>
+    <col min="9" max="9" width="12.09765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.09765625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15" style="3" customWidth="1"/>
+    <col min="12" max="12" width="16" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="11"/>
+      <c r="L6" s="12"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B8" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="C8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="9">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="7">
         <f>SUM(totalBelegung)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <f>SUM(totalGutscheine)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10">
+      <c r="F9" s="8"/>
+      <c r="G9" s="8">
         <f>SUM(selbstbehaltGemeinde)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="8">
         <f>SUM(eingabeLastenausgleich)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="7">
+        <f>SUM(totalBelegungOhneSelbstbehalt)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="8">
+        <f>SUM(totalGutscheineOhneSelbstbehalt)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="8">
+        <f>SUM(kostenFuerSelbstbehalt)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="J6:L6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
KIBON-1664 finish template and add german name for zemis excel
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
@@ -8,13 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB6F944-6BD0-4BE6-8ACF-E40FFE9896A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AEF2A1-4896-4083-A2C0-4BC99625FBC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="eingabeLastenausgleich">Data!$I$8</definedName>
+    <definedName name="kostenFuerSelbstbehalt">Data!$L$8</definedName>
+    <definedName name="selbstbehaltGemeinde">Data!$H$8</definedName>
+    <definedName name="totalBelegung">Data!$E$8</definedName>
+    <definedName name="totalBelegungOhneSelbstbehalt">Data!$J$8</definedName>
+    <definedName name="totalGutscheine">Data!$F$8</definedName>
+    <definedName name="totalGutscheineOhneSelbstbehalt">Data!$K$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -132,7 +141,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -153,6 +165,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -199,10 +218,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -216,13 +236,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -675,12 +701,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -701,18 +727,18 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -765,28 +791,28 @@
       <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="9" t="s">
         <v>30</v>
       </c>
       <c r="M8" t="s">
@@ -798,26 +824,33 @@
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="5">
+      <c r="E9" s="13">
+        <f>SUM(totalBelegung)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="14">
+        <f>SUM(totalGutscheine)</f>
         <v>0</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="5">
+      <c r="H9" s="14">
+        <f>SUM(selbstbehaltGemeinde)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="14">
+        <f>SUM(eingabeLastenausgleich)</f>
         <v>0</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="13">
+        <f>SUM(totalBelegungOhneSelbstbehalt)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="14">
+        <f>SUM(totalGutscheineOhneSelbstbehalt)</f>
         <v>0</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="14">
+        <f>SUM(kostenFuerSelbstbehalt)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KIBON-1710 change header names
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu2\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AEF2A1-4896-4083-A2C0-4BC99625FBC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BA176B-F975-4733-B9E3-C129CED7834C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,12 +71,6 @@
     <t>{selbstbehaltProHundertProzentPlatz}</t>
   </si>
   <si>
-    <t>{belegungenMitSelbstbehaltTitel}</t>
-  </si>
-  <si>
-    <t>{belegungenOhneSelbstbehaltTitel}</t>
-  </si>
-  <si>
     <t>{bfsNummerTitel}</t>
   </si>
   <si>
@@ -135,6 +129,12 @@
   </si>
   <si>
     <t>{kostenFuerSelbstbehalt}</t>
+  </si>
+  <si>
+    <t>{bgMitSelbstbehaltTitel}</t>
+  </si>
+  <si>
+    <t>{bgOhneSelbstbehaltTitel}</t>
   </si>
 </sst>
 </file>
@@ -240,12 +240,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -727,55 +727,55 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="E6" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="J7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -783,37 +783,37 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="E8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="F8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="G8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="J8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="K8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="L8" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="M8" t="s">
         <v>0</v>
@@ -824,32 +824,32 @@
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <f>SUM(totalBelegung)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <f>SUM(totalGutscheine)</f>
         <v>0</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <f>SUM(selbstbehaltGemeinde)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="13">
         <f>SUM(eingabeLastenausgleich)</f>
         <v>0</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="12">
         <f>SUM(totalBelegungOhneSelbstbehalt)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="13">
         <f>SUM(totalGutscheineOhneSelbstbehalt)</f>
         <v>0</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="13">
         <f>SUM(kostenFuerSelbstbehalt)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
KIBON-1710 add correct Erläuterung keys
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu2\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7077FE0-358F-4E02-AD3C-5D4296390E71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E9B452-C39C-4351-833A-7F84F8CE8CCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1260" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -167,9 +167,6 @@
     <t>{erlaeuterungZ9_1}</t>
   </si>
   <si>
-    <t>{erlaeuterungZ10_1}</t>
-  </si>
-  <si>
     <t>{erlaeuterungZ5_2}</t>
   </si>
   <si>
@@ -185,10 +182,13 @@
     <t>{erlaeuterungZ9_2}</t>
   </si>
   <si>
-    <t>{erlaeuterungZ10_2}</t>
-  </si>
-  <si>
     <t>{erlaeuterungZ11_2}</t>
+  </si>
+  <si>
+    <t>{erlaeuterungZ1_1}</t>
+  </si>
+  <si>
+    <t>{erlaeuterungZ1_2}</t>
   </si>
 </sst>
 </file>
@@ -297,17 +297,17 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -722,7 +722,7 @@
   <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,18 +810,18 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14" t="s">
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -943,127 +943,127 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="15" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="15" t="s">
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="15" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="15" t="s">
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
KIBON-1710 increase erlaeuterungZ10 key, since 0 seems not to work with POI
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E9B452-C39C-4351-833A-7F84F8CE8CCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CB4318-E5C9-41AE-9E3D-BD810731F514}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,10 +185,10 @@
     <t>{erlaeuterungZ11_2}</t>
   </si>
   <si>
-    <t>{erlaeuterungZ1_1}</t>
-  </si>
-  <si>
-    <t>{erlaeuterungZ1_2}</t>
+    <t>{erlaeuterungZ12_1}</t>
+  </si>
+  <si>
+    <t>{erlaeuterungZ12_2}</t>
   </si>
 </sst>
 </file>
@@ -198,7 +198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -222,6 +222,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -276,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -300,15 +320,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -721,9 +747,7 @@
   </sheetPr>
   <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -774,17 +798,17 @@
       <c r="A2" s="8"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="21" t="s">
         <v>33</v>
       </c>
     </row>
@@ -810,18 +834,18 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17" t="s">
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -938,121 +962,130 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="16" t="s">
         <v>34</v>
       </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B22" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D28" s="14"/>

</xml_diff>

<commit_message>
KIBON-2651 lastenausgleichberechnung report anpassen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichBerechnung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CB4318-E5C9-41AE-9E3D-BD810731F514}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34DCA76-BB17-4645-A4CE-54A0AC29AC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,13 +16,17 @@
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="eingabeLastenausgleich">Data!$I$12</definedName>
-    <definedName name="kostenFuerSelbstbehalt">Data!$L$12</definedName>
-    <definedName name="selbstbehaltGemeinde">Data!$H$12</definedName>
+    <definedName name="eingabeLastenausgleichMitSelbstbehalt">Data!$M$12</definedName>
+    <definedName name="kostenFuerSelbstbehalt">Data!$P$12</definedName>
+    <definedName name="selbstbehaltGemeinde">Data!$L$12</definedName>
     <definedName name="totalBelegung">Data!$E$12</definedName>
-    <definedName name="totalBelegungOhneSelbstbehalt">Data!$J$12</definedName>
+    <definedName name="totalBelegungMitSelbstbehalt">Data!$I$12</definedName>
+    <definedName name="totalBelegungOhneSelbstbehalt">Data!$N$12</definedName>
+    <definedName name="totalEingabeLastenausgleich">Data!$H$12</definedName>
     <definedName name="totalGutscheine">Data!$F$12</definedName>
-    <definedName name="totalGutscheineOhneSelbstbehalt">Data!$K$12</definedName>
+    <definedName name="totalGutscheineMitSelbstbehalt">Data!$J$12</definedName>
+    <definedName name="totalGutscheineOhneSelbstbehalt">Data!$O$12</definedName>
+    <definedName name="totalSelbstbehaltGemeinde">Data!$G$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>{repeatRow}</t>
   </si>
@@ -113,15 +117,9 @@
     <t>{totalGutscheine}</t>
   </si>
   <si>
-    <t>{kostenProHundertProzentPlatz}</t>
-  </si>
-  <si>
     <t>{selbstbehaltGemeinde}</t>
   </si>
   <si>
-    <t>{eingabeLastenausgleich}</t>
-  </si>
-  <si>
     <t>{totalBelegungOhneSelbstbehalt}</t>
   </si>
   <si>
@@ -189,6 +187,24 @@
   </si>
   <si>
     <t>{erlaeuterungZ12_2}</t>
+  </si>
+  <si>
+    <t>{bgTotalGemaessStichtagTitle}</t>
+  </si>
+  <si>
+    <t>{totalBelegungMitSelbstbehalt}</t>
+  </si>
+  <si>
+    <t>{totalGutscheineMitSelbstbehalt}</t>
+  </si>
+  <si>
+    <t>{kostenProHundertProzentPlatzMitSelbstbehalt}</t>
+  </si>
+  <si>
+    <t>{eingabeLastenausgleichMitSelbstbehalt}</t>
+  </si>
+  <si>
+    <t>{totalEingabeLastenausgleich}</t>
   </si>
 </sst>
 </file>
@@ -320,9 +336,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -331,10 +344,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -745,79 +761,78 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB28"/>
+  <dimension ref="A1:AA28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1"/>
-    <col min="15" max="15" width="22"/>
-    <col min="16" max="16" width="15.85546875" customWidth="1"/>
-    <col min="17" max="20" width="22"/>
-    <col min="25" max="26" width="12.7109375"/>
-    <col min="27" max="27" width="11.28515625" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="16" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="16" customWidth="1"/>
-    <col min="30" max="31" width="12.7109375"/>
-    <col min="32" max="32" width="12.7109375" customWidth="1"/>
-    <col min="33" max="33" width="12.28515625" customWidth="1"/>
-    <col min="34" max="34" width="16.85546875"/>
-    <col min="35" max="35" width="13.28515625" customWidth="1"/>
-    <col min="36" max="36" width="13.42578125" customWidth="1"/>
-    <col min="37" max="37" width="12.7109375"/>
-    <col min="38" max="38" width="19.42578125"/>
-    <col min="40" max="40" width="16.85546875"/>
-    <col min="41" max="42" width="12.7109375"/>
-    <col min="43" max="43" width="12.28515625" customWidth="1"/>
-    <col min="44" max="44" width="12.7109375" customWidth="1"/>
-    <col min="45" max="45" width="12.7109375"/>
-    <col min="46" max="46" width="13.5703125" customWidth="1"/>
-    <col min="47" max="1000" width="10.5703125"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625"/>
+    <col min="13" max="13" width="20.6640625" customWidth="1"/>
+    <col min="14" max="14" width="22"/>
+    <col min="15" max="15" width="15.88671875" customWidth="1"/>
+    <col min="16" max="19" width="22"/>
+    <col min="24" max="25" width="12.6640625"/>
+    <col min="26" max="26" width="11.33203125" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="16" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="16" customWidth="1"/>
+    <col min="29" max="30" width="12.6640625"/>
+    <col min="31" max="31" width="12.6640625" customWidth="1"/>
+    <col min="32" max="32" width="12.33203125" customWidth="1"/>
+    <col min="33" max="33" width="16.88671875"/>
+    <col min="34" max="34" width="13.33203125" customWidth="1"/>
+    <col min="35" max="35" width="13.44140625" customWidth="1"/>
+    <col min="36" max="36" width="12.6640625"/>
+    <col min="37" max="37" width="19.44140625"/>
+    <col min="39" max="39" width="16.88671875"/>
+    <col min="40" max="41" width="12.6640625"/>
+    <col min="42" max="42" width="12.33203125" customWidth="1"/>
+    <col min="43" max="43" width="12.6640625" customWidth="1"/>
+    <col min="44" max="44" width="12.6640625"/>
+    <col min="45" max="45" width="13.5546875" customWidth="1"/>
+    <col min="46" max="999" width="10.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="10.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -825,7 +840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -833,21 +848,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="E10" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
@@ -867,25 +888,37 @@
         <v>12</v>
       </c>
       <c r="G11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="M11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="N11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="O11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="P11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -908,25 +941,37 @@
         <v>23</v>
       </c>
       <c r="H12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="N12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="O12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="P12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="Q12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -939,155 +984,163 @@
         <f>SUM(totalGutscheine)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="13">
+        <f>SUM(totalSelbstbehaltGemeinde)</f>
+        <v>0</v>
+      </c>
       <c r="H13" s="13">
+        <f>SUM(totalEingabeLastenausgleich)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="12">
+        <f>SUM(totalBelegungMitSelbstbehalt)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="13">
+        <f>SUM(totalGutscheineMitSelbstbehalt)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="13">
         <f>SUM(selbstbehaltGemeinde)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="13">
-        <f>SUM(eingabeLastenausgleich)</f>
+      <c r="M13" s="13">
+        <f>SUM(eingabeLastenausgleichMitSelbstbehalt)</f>
         <v>0</v>
       </c>
-      <c r="J13" s="12">
+      <c r="N13" s="12">
         <f>SUM(totalBelegungOhneSelbstbehalt)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="13">
+      <c r="O13" s="13">
         <f>SUM(totalGutscheineOhneSelbstbehalt)</f>
         <v>0</v>
       </c>
-      <c r="L13" s="13">
+      <c r="P13" s="13">
         <f>SUM(kostenFuerSelbstbehalt)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="B16" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+    </row>
+    <row r="18" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B18" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-    </row>
-    <row r="18" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B20" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="20" t="s">
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="20" t="s">
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="20" t="s">
+      <c r="B22" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
@@ -1096,19 +1149,19 @@
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B18:J18"/>
+  <mergeCells count="10">
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="E10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>